<commit_message>
Exe 13 - copy
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/6.thao-tac-voi-file.xlsx
+++ b/me/1.Lap-trinh-python/6.thao-tac-voi-file.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BBF1645-4945-3E47-93FC-D15994B302B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27F3C7F-9453-BC42-83C0-7E0968E5C272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="740" windowWidth="30660" windowHeight="18920" activeTab="3" xr2:uid="{8DE6A8FB-9853-2046-B3E0-1DBE49BB7982}"/>
+    <workbookView xWindow="1260" yWindow="740" windowWidth="30660" windowHeight="18920" activeTab="4" xr2:uid="{8DE6A8FB-9853-2046-B3E0-1DBE49BB7982}"/>
   </bookViews>
   <sheets>
     <sheet name="open" sheetId="1" r:id="rId1"/>
     <sheet name="Readline" sheetId="2" r:id="rId2"/>
     <sheet name="Write" sheetId="3" r:id="rId3"/>
     <sheet name="With" sheetId="4" r:id="rId4"/>
+    <sheet name="Exe 13 - copy" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="141">
   <si>
     <t>構成</t>
   </si>
@@ -422,6 +423,45 @@
   </si>
   <si>
     <t>Với việc dùng with thì không cần dùng close()</t>
+  </si>
+  <si>
+    <t>exe_13_copy.py</t>
+  </si>
+  <si>
+    <t>python/exe/exe_13_copy.py</t>
+  </si>
+  <si>
+    <t>data</t>
+  </si>
+  <si>
+    <t>abc.txt</t>
+  </si>
+  <si>
+    <t>def.txt</t>
+  </si>
+  <si>
+    <t>python/exe/data/abc.txt</t>
+  </si>
+  <si>
+    <t>from shutil import copyfile</t>
+  </si>
+  <si>
+    <t>fileOne = "data/abc.txt"</t>
+  </si>
+  <si>
+    <t>fileTwo = "data/def.txt"</t>
+  </si>
+  <si>
+    <t>copyfile(fileOne, fileTwo)</t>
+  </si>
+  <si>
+    <t>python3 exe_13_copy.py</t>
+  </si>
+  <si>
+    <t>python/exe/data/def.txt</t>
+  </si>
+  <si>
+    <t>Check def.txt</t>
   </si>
 </sst>
 </file>
@@ -1463,6 +1503,108 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121337</xdr:colOff>
+      <xdr:row>77</xdr:row>
+      <xdr:rowOff>88981</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>379576</xdr:colOff>
+      <xdr:row>81</xdr:row>
+      <xdr:rowOff>64714</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E3BA677-7C6F-A32A-0CA6-124839D5138C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="946433" y="15660637"/>
+          <a:ext cx="9334289" cy="784650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>135467</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>16933</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>491067</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CB580F9B-DAE3-92BD-CB07-BF47C397FC48}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="965200" y="12818533"/>
+          <a:ext cx="355600" cy="4656667"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -4594,8 +4736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0554C847-1E9F-7B46-8BEC-52F344C854F3}">
   <dimension ref="A3:L75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G60" sqref="G60"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:H52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4986,7 +5128,7 @@
       <c r="A35" s="6"/>
       <c r="B35" s="15"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="23" t="s">
+      <c r="D35" t="s">
         <v>102</v>
       </c>
       <c r="E35" s="7"/>
@@ -5221,38 +5363,28 @@
       <c r="B57" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="C57" s="24"/>
-      <c r="D57" s="24"/>
       <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B58" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="C58" s="24"/>
-      <c r="D58" s="24"/>
       <c r="E58" s="5"/>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
-      <c r="C59" s="24"/>
-      <c r="D59" s="24"/>
       <c r="E59" s="5"/>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B60" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C60" s="24"/>
-      <c r="D60" s="24"/>
       <c r="E60" s="5"/>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B61" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="C61" s="24"/>
-      <c r="D61" s="24"/>
       <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
@@ -5278,119 +5410,38 @@
     </row>
     <row r="66" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
-      <c r="C66" s="24"/>
-      <c r="D66" s="24"/>
-      <c r="E66" s="24"/>
-      <c r="F66" s="24"/>
-      <c r="G66" s="24"/>
-      <c r="H66" s="24"/>
-      <c r="I66" s="24"/>
-      <c r="J66" s="24"/>
-      <c r="K66" s="24"/>
       <c r="L66" s="5"/>
     </row>
     <row r="67" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B67" s="4"/>
-      <c r="C67" s="24"/>
-      <c r="D67" s="24"/>
-      <c r="E67" s="24"/>
-      <c r="F67" s="24"/>
-      <c r="G67" s="24"/>
-      <c r="H67" s="24"/>
-      <c r="I67" s="24"/>
-      <c r="J67" s="24"/>
-      <c r="K67" s="24"/>
       <c r="L67" s="5"/>
     </row>
     <row r="68" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="24"/>
-      <c r="J68" s="24"/>
-      <c r="K68" s="24"/>
       <c r="L68" s="5"/>
     </row>
     <row r="69" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B69" s="4"/>
-      <c r="C69" s="24"/>
-      <c r="D69" s="24"/>
-      <c r="E69" s="24"/>
-      <c r="F69" s="24"/>
-      <c r="G69" s="24"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="24"/>
-      <c r="J69" s="24"/>
-      <c r="K69" s="24"/>
       <c r="L69" s="5"/>
     </row>
     <row r="70" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B70" s="4"/>
-      <c r="C70" s="24"/>
-      <c r="D70" s="24"/>
-      <c r="E70" s="24"/>
-      <c r="F70" s="24"/>
-      <c r="G70" s="24"/>
-      <c r="H70" s="24"/>
-      <c r="I70" s="24"/>
-      <c r="J70" s="24"/>
-      <c r="K70" s="24"/>
       <c r="L70" s="5"/>
     </row>
     <row r="71" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="24"/>
-      <c r="D71" s="24"/>
-      <c r="E71" s="24"/>
-      <c r="F71" s="24"/>
-      <c r="G71" s="24"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="24"/>
-      <c r="J71" s="24"/>
-      <c r="K71" s="24"/>
       <c r="L71" s="5"/>
     </row>
     <row r="72" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B72" s="4"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="24"/>
-      <c r="E72" s="24"/>
-      <c r="F72" s="24"/>
-      <c r="G72" s="24"/>
-      <c r="H72" s="24"/>
-      <c r="I72" s="24"/>
-      <c r="J72" s="24"/>
-      <c r="K72" s="24"/>
       <c r="L72" s="5"/>
     </row>
     <row r="73" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B73" s="4"/>
-      <c r="C73" s="24"/>
-      <c r="D73" s="24"/>
-      <c r="E73" s="24"/>
-      <c r="F73" s="24"/>
-      <c r="G73" s="24"/>
-      <c r="H73" s="24"/>
-      <c r="I73" s="24"/>
-      <c r="J73" s="24"/>
-      <c r="K73" s="24"/>
       <c r="L73" s="5"/>
     </row>
     <row r="74" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B74" s="4"/>
-      <c r="C74" s="24"/>
-      <c r="D74" s="24"/>
-      <c r="E74" s="24"/>
-      <c r="F74" s="24"/>
-      <c r="G74" s="24"/>
-      <c r="H74" s="24"/>
-      <c r="I74" s="24"/>
-      <c r="J74" s="24"/>
-      <c r="K74" s="24"/>
       <c r="L74" s="5"/>
     </row>
     <row r="75" spans="2:12" x14ac:dyDescent="0.2">
@@ -5410,4 +5461,880 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2236F8-61C0-0B4F-8696-65159BCD898C}">
+  <dimension ref="A3:M90"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B93" sqref="B93"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="6"/>
+      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="6"/>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="16"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="6"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="6"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="6"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="6"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="6"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="6"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="6"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="6"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="6"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="6"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H55" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="6"/>
+      <c r="B56" s="18"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="19"/>
+      <c r="E56" s="19"/>
+      <c r="F56" s="20"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B60" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C60" s="3"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B61" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C61" s="5"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B62" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C62" s="5"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B63" s="8"/>
+      <c r="C63" s="10"/>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A66" s="22" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B67" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="3"/>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B68" s="4"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="5"/>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B69" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="C69" s="24"/>
+      <c r="D69" s="5"/>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B70" s="4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C70" s="24"/>
+      <c r="D70" s="5"/>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B71" s="4"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="5"/>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B72" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C72" s="24"/>
+      <c r="D72" s="5"/>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B73" s="8"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="10"/>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A76" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B76" s="2"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+      <c r="E76" s="2"/>
+      <c r="F76" s="2"/>
+      <c r="G76" s="2"/>
+      <c r="H76" s="2"/>
+      <c r="I76" s="2"/>
+      <c r="J76" s="2"/>
+      <c r="K76" s="2"/>
+      <c r="L76" s="2"/>
+      <c r="M76" s="3"/>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A77" s="4"/>
+      <c r="B77" s="24" t="s">
+        <v>138</v>
+      </c>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="24"/>
+      <c r="K77" s="24"/>
+      <c r="L77" s="24"/>
+      <c r="M77" s="5"/>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A78" s="4"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="24"/>
+      <c r="L78" s="24"/>
+      <c r="M78" s="5"/>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A79" s="4"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+      <c r="K79" s="24"/>
+      <c r="L79" s="24"/>
+      <c r="M79" s="5"/>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A80" s="4"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="24"/>
+      <c r="L80" s="24"/>
+      <c r="M80" s="5"/>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A81" s="4"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24"/>
+      <c r="K81" s="24"/>
+      <c r="L81" s="24"/>
+      <c r="M81" s="5"/>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A82" s="8"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="9"/>
+      <c r="D82" s="9"/>
+      <c r="E82" s="9"/>
+      <c r="F82" s="9"/>
+      <c r="G82" s="9"/>
+      <c r="H82" s="9"/>
+      <c r="I82" s="9"/>
+      <c r="J82" s="9"/>
+      <c r="K82" s="9"/>
+      <c r="L82" s="9"/>
+      <c r="M82" s="10"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A85" s="22" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B86" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B87" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C87" s="3"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B88" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C88" s="5"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B89" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C89" s="5"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B90" s="8"/>
+      <c r="C90" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Exe 14 - student
</commit_message>
<xml_diff>
--- a/me/1.Lap-trinh-python/6.thao-tac-voi-file.xlsx
+++ b/me/1.Lap-trinh-python/6.thao-tac-voi-file.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vudinhquang/Documents/quang/python/me/1.Lap-trinh-python/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F27F3C7F-9453-BC42-83C0-7E0968E5C272}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB0CE592-2E19-C845-8455-397D60317740}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1260" yWindow="740" windowWidth="30660" windowHeight="18920" activeTab="4" xr2:uid="{8DE6A8FB-9853-2046-B3E0-1DBE49BB7982}"/>
+    <workbookView xWindow="1260" yWindow="740" windowWidth="30660" windowHeight="18920" activeTab="5" xr2:uid="{8DE6A8FB-9853-2046-B3E0-1DBE49BB7982}"/>
   </bookViews>
   <sheets>
     <sheet name="open" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Write" sheetId="3" r:id="rId3"/>
     <sheet name="With" sheetId="4" r:id="rId4"/>
     <sheet name="Exe 13 - copy" sheetId="5" r:id="rId5"/>
+    <sheet name="Exe 14 - student" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="534" uniqueCount="197">
   <si>
     <t>構成</t>
   </si>
@@ -462,6 +463,174 @@
   </si>
   <si>
     <t>Check def.txt</t>
+  </si>
+  <si>
+    <t>exe_14_student.py</t>
+  </si>
+  <si>
+    <t>info.txt</t>
+  </si>
+  <si>
+    <t>score.txt</t>
+  </si>
+  <si>
+    <t>student.txt</t>
+  </si>
+  <si>
+    <t>python/exe/exe_14_student.py</t>
+  </si>
+  <si>
+    <t>import json</t>
+  </si>
+  <si>
+    <t>fileOne     = "data/info.txt"</t>
+  </si>
+  <si>
+    <t>fileTwo     = "data/score.txt"</t>
+  </si>
+  <si>
+    <t>fileStudent = "data/student.txt"</t>
+  </si>
+  <si>
+    <t>data    = []</t>
+  </si>
+  <si>
+    <t>with open(fileOne) as fileInfo, open(fileTwo) as fileScore:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    for lineInfo, lineScore in zip(fileInfo,fileScore):</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        data.append({</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            'name': lineInfo.rstrip(),</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            'score': lineScore.rstrip()</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        })</t>
+  </si>
+  <si>
+    <t>with open(fileStudent, 'w') as fileStudentObj:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    fileStudentObj.write(json.dumps(data)) </t>
+  </si>
+  <si>
+    <t>data = ""</t>
+  </si>
+  <si>
+    <t>with open(fileStudent, 'r') as fileStudentObj:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    data = fileStudentObj.read()</t>
+  </si>
+  <si>
+    <t>result = json.loads(data)</t>
+  </si>
+  <si>
+    <t>for info in result:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print ("- Name: {}\n- Score: {}".format(</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        info["name"],</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        info["score"]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    ))</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    print("-------------------------")</t>
+  </si>
+  <si>
+    <t>python/exe/data/info.txt</t>
+  </si>
+  <si>
+    <t>vuquang</t>
+  </si>
+  <si>
+    <t>dinhquang</t>
+  </si>
+  <si>
+    <t>quangvu</t>
+  </si>
+  <si>
+    <t>python/exe/data/score.txt</t>
+  </si>
+  <si>
+    <t>8,9</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>zip: Loop cho cả fileInfo và fileScore cùng 1 lúc</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>rstrip(): Xoá \n</t>
+  </si>
+  <si>
+    <t>json.dumps(data): Chuyển data sang chuỗi json</t>
+  </si>
+  <si>
+    <t>json.loads(data): Chuyển chuỗi dạng json sang List</t>
+  </si>
+  <si>
+    <t>python3 exe_14_student.py</t>
+  </si>
+  <si>
+    <t>[{"name": "vuquang", "score": "8,9"}, {"name": "dinhquang", "score": "1,2"}, {"name": "quangvu", "score": "3,4"}]</t>
+  </si>
+  <si>
+    <t>&lt;class 'str'&gt;</t>
+  </si>
+  <si>
+    <t>print(result)</t>
+  </si>
+  <si>
+    <t>print(type(result))</t>
+  </si>
+  <si>
+    <t>[{'name': 'vuquang', 'score': '8,9'}, {'name': 'dinhquang', 'score': '1,2'}, {'name': 'quangvu', 'score': '3,4'}]</t>
+  </si>
+  <si>
+    <t>- Name: vuquang</t>
+  </si>
+  <si>
+    <t>- Score: 8,9</t>
+  </si>
+  <si>
+    <t>-------------------------</t>
+  </si>
+  <si>
+    <t>- Name: dinhquang</t>
+  </si>
+  <si>
+    <t>- Score: 1,2</t>
+  </si>
+  <si>
+    <t>- Name: quangvu</t>
+  </si>
+  <si>
+    <t>- Score: 3,4</t>
+  </si>
+  <si>
+    <t>Check student.txt</t>
+  </si>
+  <si>
+    <t>python/exe/data/student.txt</t>
   </si>
 </sst>
 </file>
@@ -630,7 +799,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1605,6 +1776,214 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>375920</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="3" name="Straight Arrow Connector 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89887ADC-D839-BC67-E4B5-8ABAD5C929A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2560320" y="17221200"/>
+          <a:ext cx="284480" cy="132080"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>142240</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>172720</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>812800</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B095E2B-25F8-5713-A14B-9AD9EF54C855}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1">
+          <a:off x="3434080" y="17241520"/>
+          <a:ext cx="670560" cy="111760"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>91439</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>131076</xdr:colOff>
+      <xdr:row>132</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AEEF1819-0A52-9DF2-9808-7565BEEC5D45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="914399" y="23449280"/>
+          <a:ext cx="9915157" cy="2987040"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>416560</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>538480</xdr:colOff>
+      <xdr:row>136</xdr:row>
+      <xdr:rowOff>81280</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Arrow Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{035A1D0E-539D-6F30-3046-0FE5FA3503D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2062480" y="18877280"/>
+          <a:ext cx="121920" cy="8839200"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -5467,8 +5846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF2236F8-61C0-0B4F-8696-65159BCD898C}">
   <dimension ref="A3:M90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5869,7 +6248,7 @@
       <c r="A36" s="6"/>
       <c r="B36" s="15"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="23" t="s">
+      <c r="D36" t="s">
         <v>119</v>
       </c>
       <c r="E36" s="7"/>
@@ -5920,8 +6299,12 @@
       </c>
       <c r="E40" s="6"/>
       <c r="F40" s="16"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
+      <c r="G40" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="6"/>
@@ -5932,8 +6315,12 @@
       </c>
       <c r="E41" s="6"/>
       <c r="F41" s="16"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
+      <c r="G41" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="6"/>
@@ -6158,33 +6545,28 @@
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B68" s="4"/>
-      <c r="C68" s="24"/>
       <c r="D68" s="5"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B69" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C69" s="24"/>
       <c r="D69" s="5"/>
     </row>
     <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B70" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="C70" s="24"/>
       <c r="D70" s="5"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B71" s="4"/>
-      <c r="C71" s="24"/>
       <c r="D71" s="5"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B72" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C72" s="24"/>
       <c r="D72" s="5"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.2">
@@ -6211,79 +6593,25 @@
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" s="4"/>
-      <c r="B77" s="24" t="s">
+      <c r="B77" t="s">
         <v>138</v>
       </c>
-      <c r="C77" s="24"/>
-      <c r="D77" s="24"/>
-      <c r="E77" s="24"/>
-      <c r="F77" s="24"/>
-      <c r="G77" s="24"/>
-      <c r="H77" s="24"/>
-      <c r="I77" s="24"/>
-      <c r="J77" s="24"/>
-      <c r="K77" s="24"/>
-      <c r="L77" s="24"/>
       <c r="M77" s="5"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" s="4"/>
-      <c r="B78" s="24"/>
-      <c r="C78" s="24"/>
-      <c r="D78" s="24"/>
-      <c r="E78" s="24"/>
-      <c r="F78" s="24"/>
-      <c r="G78" s="24"/>
-      <c r="H78" s="24"/>
-      <c r="I78" s="24"/>
-      <c r="J78" s="24"/>
-      <c r="K78" s="24"/>
-      <c r="L78" s="24"/>
       <c r="M78" s="5"/>
     </row>
     <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" s="4"/>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
-      <c r="D79" s="24"/>
-      <c r="E79" s="24"/>
-      <c r="F79" s="24"/>
-      <c r="G79" s="24"/>
-      <c r="H79" s="24"/>
-      <c r="I79" s="24"/>
-      <c r="J79" s="24"/>
-      <c r="K79" s="24"/>
-      <c r="L79" s="24"/>
       <c r="M79" s="5"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" s="4"/>
-      <c r="B80" s="24"/>
-      <c r="C80" s="24"/>
-      <c r="D80" s="24"/>
-      <c r="E80" s="24"/>
-      <c r="F80" s="24"/>
-      <c r="G80" s="24"/>
-      <c r="H80" s="24"/>
-      <c r="I80" s="24"/>
-      <c r="J80" s="24"/>
-      <c r="K80" s="24"/>
-      <c r="L80" s="24"/>
       <c r="M80" s="5"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" s="4"/>
-      <c r="B81" s="24"/>
-      <c r="C81" s="24"/>
-      <c r="D81" s="24"/>
-      <c r="E81" s="24"/>
-      <c r="F81" s="24"/>
-      <c r="G81" s="24"/>
-      <c r="H81" s="24"/>
-      <c r="I81" s="24"/>
-      <c r="J81" s="24"/>
-      <c r="K81" s="24"/>
-      <c r="L81" s="24"/>
       <c r="M81" s="5"/>
     </row>
     <row r="82" spans="1:13" x14ac:dyDescent="0.2">
@@ -6337,4 +6665,1366 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8BE2D19-7B0D-2D4E-9AE3-8F092C2282C9}">
+  <dimension ref="A3:N140"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C141" sqref="C141"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="6"/>
+      <c r="B4" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13"/>
+      <c r="E4" s="13"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="6"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="16"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="6"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="16"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="6"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="16"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" s="6"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="6"/>
+      <c r="F8" s="16"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="6"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" s="6"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="6"/>
+      <c r="B10" s="15"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="6"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="6"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="6"/>
+      <c r="F11" s="16"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="6"/>
+      <c r="B12" s="15"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="6"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6"/>
+      <c r="B13" s="15"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="6"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6"/>
+      <c r="B14" s="15"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="6"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="6"/>
+      <c r="B15" s="15"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="6"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="6"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="6"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="6"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="6"/>
+      <c r="F17" s="16"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" s="6"/>
+      <c r="B18" s="15"/>
+      <c r="C18" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="17"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="6"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="6"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="6"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="6"/>
+      <c r="D20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E20" s="6"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" s="6"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="6"/>
+      <c r="D21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E21" s="6"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="6"/>
+      <c r="H21" s="6"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" s="6"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" s="6"/>
+      <c r="F22" s="16"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" s="6"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" s="6"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="16"/>
+      <c r="G23" s="6"/>
+      <c r="H23" s="6"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" s="6"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="6"/>
+      <c r="D24" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="16"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="6"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" s="6"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="6"/>
+      <c r="F25" s="16"/>
+      <c r="G25" s="6"/>
+      <c r="H25" s="6"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" s="6"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="16"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="6"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E27" s="6"/>
+      <c r="F27" s="16"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" s="6"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E28" s="6"/>
+      <c r="F28" s="16"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" s="6"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="16"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" s="6"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="6"/>
+      <c r="D30" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A31" s="6"/>
+      <c r="B31" s="15"/>
+      <c r="C31" s="6"/>
+      <c r="D31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="6"/>
+      <c r="F31" s="16"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A32" s="6"/>
+      <c r="B32" s="15"/>
+      <c r="C32" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="16"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="6"/>
+      <c r="B33" s="15"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="E33" s="6"/>
+      <c r="F33" s="16"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="6"/>
+      <c r="B34" s="15"/>
+      <c r="C34" s="6"/>
+      <c r="D34" t="s">
+        <v>78</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="16"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="6"/>
+      <c r="B35" s="15"/>
+      <c r="C35" s="6"/>
+      <c r="D35" t="s">
+        <v>102</v>
+      </c>
+      <c r="E35" s="7"/>
+      <c r="F35" s="16"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="6"/>
+      <c r="B36" s="15"/>
+      <c r="C36" s="6"/>
+      <c r="D36" t="s">
+        <v>119</v>
+      </c>
+      <c r="E36" s="7"/>
+      <c r="F36" s="16"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="6"/>
+      <c r="B37" s="15"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="6"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A38" s="6"/>
+      <c r="B38" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A39" s="6"/>
+      <c r="B39" s="15"/>
+      <c r="C39" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A40" s="6"/>
+      <c r="B40" s="15"/>
+      <c r="C40" s="6"/>
+      <c r="D40" t="s">
+        <v>131</v>
+      </c>
+      <c r="E40" s="6"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A41" s="6"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="6"/>
+      <c r="D41" t="s">
+        <v>132</v>
+      </c>
+      <c r="E41" s="6"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A42" s="6"/>
+      <c r="B42" s="15"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E42" s="6"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A43" s="6"/>
+      <c r="B43" s="15"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="E43" s="6"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" s="6"/>
+      <c r="B44" s="15"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="E44" s="6"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="6"/>
+      <c r="B45" s="15"/>
+      <c r="C45" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="6"/>
+      <c r="B46" s="15"/>
+      <c r="C46" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="6"/>
+      <c r="B47" s="15"/>
+      <c r="C47" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="6"/>
+      <c r="B48" s="15"/>
+      <c r="C48" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="6"/>
+      <c r="B49" s="15"/>
+      <c r="C49" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="6"/>
+      <c r="B50" s="15"/>
+      <c r="C50" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="6"/>
+      <c r="B51" s="15"/>
+      <c r="C51" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="6"/>
+      <c r="B52" s="15"/>
+      <c r="C52" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="6"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A54" s="6"/>
+      <c r="B54" s="15"/>
+      <c r="C54" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="6"/>
+      <c r="B55" s="15"/>
+      <c r="C55" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="6"/>
+      <c r="B56" s="15"/>
+      <c r="C56" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="6"/>
+      <c r="B57" s="15"/>
+      <c r="C57" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="6"/>
+      <c r="B58" s="15"/>
+      <c r="C58" t="s">
+        <v>128</v>
+      </c>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="16"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="6"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H59" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="6"/>
+      <c r="B60" s="18"/>
+      <c r="C60" s="19"/>
+      <c r="D60" s="19"/>
+      <c r="E60" s="19"/>
+      <c r="F60" s="20"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="6"/>
+      <c r="B61" s="6"/>
+      <c r="C61" s="6"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="6"/>
+      <c r="B62" s="6"/>
+      <c r="C62" s="6"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="6"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="6"/>
+      <c r="B64" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="C64" s="14"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="6"/>
+      <c r="B65" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C65" s="16"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="6"/>
+      <c r="B66" s="15" t="s">
+        <v>172</v>
+      </c>
+      <c r="C66" s="16"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="6"/>
+      <c r="B67" s="18"/>
+      <c r="C67" s="20"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="6"/>
+      <c r="B68" s="6"/>
+      <c r="C68" s="6"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="6"/>
+      <c r="B69" s="6"/>
+      <c r="C69" s="6"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="6"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="6"/>
+      <c r="B71" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="C71" s="14"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="6"/>
+      <c r="B72" s="15" t="s">
+        <v>175</v>
+      </c>
+      <c r="C72" s="16"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="6"/>
+      <c r="B73" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="C73" s="16"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="6"/>
+      <c r="B74" s="18"/>
+      <c r="C74" s="20"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="6"/>
+      <c r="B75" s="6"/>
+      <c r="C75" s="6"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B78" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="2"/>
+      <c r="D78" s="2"/>
+      <c r="E78" s="2"/>
+      <c r="F78" s="3"/>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B79" s="4"/>
+      <c r="F79" s="5"/>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B80" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F80" s="5"/>
+    </row>
+    <row r="81" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B81" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="F81" s="5"/>
+    </row>
+    <row r="82" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B82" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="F82" s="5"/>
+    </row>
+    <row r="83" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B83" s="4"/>
+      <c r="F83" s="5"/>
+    </row>
+    <row r="84" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B84" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="F84" s="5"/>
+      <c r="G84" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H84" s="23" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="85" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B85" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F85" s="5"/>
+    </row>
+    <row r="86" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B86" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="F86" s="5"/>
+      <c r="G86" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H86" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="87" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B87" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B88" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="F88" s="5"/>
+      <c r="G88" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H88" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B89" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="F89" s="5"/>
+      <c r="G89" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H89" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="90" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B90" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="F90" s="5"/>
+    </row>
+    <row r="91" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B91" s="4"/>
+      <c r="F91" s="5"/>
+    </row>
+    <row r="92" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B92" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="F92" s="5"/>
+    </row>
+    <row r="93" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B93" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="F93" s="5"/>
+      <c r="G93" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H93" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="94" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B94" s="4"/>
+      <c r="F94" s="5"/>
+    </row>
+    <row r="95" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B95" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F95" s="5"/>
+    </row>
+    <row r="96" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B96" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="F96" s="5"/>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B97" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="F97" s="5"/>
+    </row>
+    <row r="98" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B98" s="4"/>
+      <c r="F98" s="5"/>
+    </row>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B99" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="F99" s="5"/>
+      <c r="G99" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H99" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="100" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B100" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="F100" s="5"/>
+      <c r="G100" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H100" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="101" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B101" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="F101" s="5"/>
+      <c r="G101" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H101" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="102" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B102" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="F102" s="5"/>
+      <c r="G102" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H102" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="103" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B103" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="F103" s="5"/>
+      <c r="G103" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H103" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B104" s="4"/>
+      <c r="F104" s="5"/>
+    </row>
+    <row r="105" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B105" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="F105" s="5"/>
+      <c r="G105" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="I105" s="2"/>
+      <c r="J105" s="3"/>
+    </row>
+    <row r="106" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B106" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="F106" s="5"/>
+      <c r="H106" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="J106" s="5"/>
+    </row>
+    <row r="107" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B107" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F107" s="5"/>
+      <c r="H107" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J107" s="5"/>
+    </row>
+    <row r="108" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B108" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="F108" s="5"/>
+      <c r="H108" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="J108" s="5"/>
+    </row>
+    <row r="109" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B109" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="F109" s="5"/>
+      <c r="H109" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="J109" s="5"/>
+    </row>
+    <row r="110" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B110" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="F110" s="5"/>
+      <c r="H110" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="J110" s="5"/>
+    </row>
+    <row r="111" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="B111" s="8"/>
+      <c r="C111" s="9"/>
+      <c r="D111" s="9"/>
+      <c r="E111" s="9"/>
+      <c r="F111" s="10"/>
+      <c r="H111" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="J111" s="5"/>
+    </row>
+    <row r="112" spans="2:10" x14ac:dyDescent="0.2">
+      <c r="H112" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="J112" s="5"/>
+    </row>
+    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H113" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="I113" s="9"/>
+      <c r="J113" s="10"/>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A116" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B116" s="2"/>
+      <c r="C116" s="2"/>
+      <c r="D116" s="2"/>
+      <c r="E116" s="2"/>
+      <c r="F116" s="2"/>
+      <c r="G116" s="2"/>
+      <c r="H116" s="2"/>
+      <c r="I116" s="2"/>
+      <c r="J116" s="2"/>
+      <c r="K116" s="2"/>
+      <c r="L116" s="2"/>
+      <c r="M116" s="2"/>
+      <c r="N116" s="3"/>
+    </row>
+    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A117" s="4"/>
+      <c r="B117" t="s">
+        <v>182</v>
+      </c>
+      <c r="N117" s="5"/>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A118" s="4"/>
+      <c r="N118" s="5"/>
+    </row>
+    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A119" s="4"/>
+      <c r="N119" s="5"/>
+    </row>
+    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A120" s="4"/>
+      <c r="N120" s="5"/>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A121" s="4"/>
+      <c r="N121" s="5"/>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A122" s="4"/>
+      <c r="N122" s="5"/>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A123" s="4"/>
+      <c r="N123" s="5"/>
+    </row>
+    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A124" s="4"/>
+      <c r="N124" s="5"/>
+    </row>
+    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A125" s="4"/>
+      <c r="N125" s="5"/>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A126" s="4"/>
+      <c r="N126" s="5"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A127" s="4"/>
+      <c r="N127" s="5"/>
+    </row>
+    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A128" s="4"/>
+      <c r="N128" s="5"/>
+    </row>
+    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A129" s="4"/>
+      <c r="N129" s="5"/>
+    </row>
+    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A130" s="4"/>
+      <c r="N130" s="5"/>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A131" s="4"/>
+      <c r="N131" s="5"/>
+    </row>
+    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A132" s="4"/>
+      <c r="N132" s="5"/>
+    </row>
+    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A133" s="8"/>
+      <c r="B133" s="9"/>
+      <c r="C133" s="9"/>
+      <c r="D133" s="9"/>
+      <c r="E133" s="9"/>
+      <c r="F133" s="9"/>
+      <c r="G133" s="9"/>
+      <c r="H133" s="9"/>
+      <c r="I133" s="9"/>
+      <c r="J133" s="9"/>
+      <c r="K133" s="9"/>
+      <c r="L133" s="9"/>
+      <c r="M133" s="9"/>
+      <c r="N133" s="10"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A136" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="B136" s="2"/>
+      <c r="C136" s="2"/>
+      <c r="D136" s="2"/>
+      <c r="E136" s="2"/>
+      <c r="F136" s="2"/>
+      <c r="G136" s="2"/>
+      <c r="H136" s="2"/>
+      <c r="I136" s="2"/>
+      <c r="J136" s="2"/>
+      <c r="K136" s="3"/>
+    </row>
+    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A137" s="4"/>
+      <c r="B137" s="24" t="s">
+        <v>196</v>
+      </c>
+      <c r="C137" s="24"/>
+      <c r="D137" s="24"/>
+      <c r="E137" s="24"/>
+      <c r="F137" s="24"/>
+      <c r="G137" s="24"/>
+      <c r="H137" s="24"/>
+      <c r="I137" s="24"/>
+      <c r="J137" s="24"/>
+      <c r="K137" s="5"/>
+    </row>
+    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A138" s="4"/>
+      <c r="B138" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C138" s="2"/>
+      <c r="D138" s="2"/>
+      <c r="E138" s="2"/>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2"/>
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
+      <c r="J138" s="3"/>
+      <c r="K138" s="5"/>
+    </row>
+    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A139" s="4"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="9"/>
+      <c r="D139" s="9"/>
+      <c r="E139" s="9"/>
+      <c r="F139" s="9"/>
+      <c r="G139" s="9"/>
+      <c r="H139" s="9"/>
+      <c r="I139" s="9"/>
+      <c r="J139" s="10"/>
+      <c r="K139" s="5"/>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A140" s="8"/>
+      <c r="B140" s="9"/>
+      <c r="C140" s="9"/>
+      <c r="D140" s="9"/>
+      <c r="E140" s="9"/>
+      <c r="F140" s="9"/>
+      <c r="G140" s="9"/>
+      <c r="H140" s="9"/>
+      <c r="I140" s="9"/>
+      <c r="J140" s="9"/>
+      <c r="K140" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>